<commit_message>
Create test notebook for request generation and sample request dataset
</commit_message>
<xml_diff>
--- a/Src/Results/Request_distribution_instance_0_demand_high.xlsx
+++ b/Src/Results/Request_distribution_instance_0_demand_high.xlsx
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -565,13 +565,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -603,13 +603,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -736,13 +736,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -793,13 +793,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -812,13 +812,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -888,13 +888,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -907,13 +907,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -945,13 +945,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -983,13 +983,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1002,13 +1002,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1059,13 +1059,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1078,10 +1078,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1192,13 +1192,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1230,10 +1230,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -1268,13 +1268,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1287,10 +1287,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -1306,10 +1306,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -1363,10 +1363,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -1382,13 +1382,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1439,10 +1439,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -1553,13 +1553,13 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -1686,13 +1686,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1705,13 +1705,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1743,13 +1743,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1838,10 +1838,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -1914,13 +1914,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -1952,10 +1952,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -1971,10 +1971,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -1990,13 +1990,13 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -2047,13 +2047,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -2142,13 +2142,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2161,13 +2161,13 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -2237,13 +2237,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -2256,13 +2256,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -2370,10 +2370,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -2389,13 +2389,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -2446,13 +2446,13 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2579,13 +2579,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -2636,13 +2636,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -2674,13 +2674,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
@@ -2693,13 +2693,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -2712,13 +2712,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D120" t="n">
         <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -2807,10 +2807,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
@@ -2883,10 +2883,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129" t="n">
         <v>0</v>
@@ -2921,13 +2921,13 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -2940,13 +2940,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -2978,13 +2978,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -3111,13 +3111,13 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -3149,13 +3149,13 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -3168,13 +3168,13 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -3206,10 +3206,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E146" t="n">
         <v>0</v>
@@ -3225,10 +3225,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E147" t="n">
         <v>0</v>
@@ -3301,13 +3301,13 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -3320,13 +3320,13 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D152" t="n">
         <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -3396,13 +3396,13 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -3548,13 +3548,13 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D164" t="n">
         <v>0</v>
       </c>
       <c r="E164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -3567,13 +3567,13 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D165" t="n">
         <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -3605,13 +3605,13 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D167" t="n">
         <v>0</v>
       </c>
       <c r="E167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -3643,13 +3643,13 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D169" t="n">
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
@@ -3662,10 +3662,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E170" t="n">
         <v>0</v>
@@ -3700,10 +3700,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E172" t="n">
         <v>0</v>
@@ -3738,13 +3738,13 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D174" t="n">
         <v>0</v>
       </c>
       <c r="E174" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -3852,10 +3852,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E180" t="n">
         <v>0</v>
@@ -3909,13 +3909,13 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -3966,13 +3966,13 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D186" t="n">
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -4061,13 +4061,13 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D191" t="n">
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -4118,10 +4118,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E194" t="n">
         <v>0</v>
@@ -4194,13 +4194,13 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -4213,10 +4213,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E199" t="n">
         <v>0</v>
@@ -4251,13 +4251,13 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D201" t="n">
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -4384,10 +4384,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E208" t="n">
         <v>0</v>
@@ -4460,13 +4460,13 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213">
@@ -4517,13 +4517,13 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D215" t="n">
         <v>0</v>
       </c>
       <c r="E215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">
@@ -4536,13 +4536,13 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D216" t="n">
         <v>0</v>
       </c>
       <c r="E216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -4574,10 +4574,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E218" t="n">
         <v>0</v>
@@ -4631,13 +4631,13 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D221" t="n">
         <v>0</v>
       </c>
       <c r="E221" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -4764,13 +4764,13 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D228" t="n">
         <v>0</v>
       </c>
       <c r="E228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -4783,10 +4783,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E229" t="n">
         <v>0</v>
@@ -5011,13 +5011,13 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D241" t="n">
         <v>0</v>
       </c>
       <c r="E241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -5068,13 +5068,13 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D244" t="n">
         <v>0</v>
       </c>
       <c r="E244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -5201,10 +5201,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E251" t="n">
         <v>0</v>
@@ -5261,10 +5261,10 @@
         <v>1</v>
       </c>
       <c r="D254" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255">
@@ -5277,10 +5277,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E255" t="n">
         <v>0</v>
@@ -5391,13 +5391,13 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D261" t="n">
         <v>0</v>
       </c>
       <c r="E261" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
@@ -5486,13 +5486,13 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D266" t="n">
         <v>0</v>
       </c>
       <c r="E266" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267">
@@ -5524,13 +5524,13 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D268" t="n">
         <v>0</v>
       </c>
       <c r="E268" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -5562,13 +5562,13 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D270" t="n">
         <v>0</v>
       </c>
       <c r="E270" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -5638,13 +5638,13 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D274" t="n">
         <v>0</v>
       </c>
       <c r="E274" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="275">
@@ -5771,13 +5771,13 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D281" t="n">
         <v>0</v>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282">
@@ -5809,13 +5809,13 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D283" t="n">
         <v>0</v>
       </c>
       <c r="E283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284">
@@ -5847,13 +5847,13 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D285" t="n">
         <v>0</v>
       </c>
       <c r="E285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286">
@@ -5885,10 +5885,10 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E287" t="n">
         <v>0</v>
@@ -5942,10 +5942,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E290" t="n">
         <v>0</v>
@@ -5980,10 +5980,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E292" t="n">
         <v>0</v>
@@ -6018,13 +6018,13 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D294" t="n">
         <v>0</v>
       </c>
       <c r="E294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
@@ -6075,13 +6075,13 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D297" t="n">
         <v>0</v>
       </c>
       <c r="E297" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298">
@@ -6113,13 +6113,13 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D299" t="n">
         <v>0</v>
       </c>
       <c r="E299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
@@ -6170,10 +6170,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D302" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E302" t="n">
         <v>0</v>
@@ -6208,13 +6208,13 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D304" t="n">
         <v>0</v>
       </c>
       <c r="E304" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305">
@@ -6322,13 +6322,13 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
@@ -6341,10 +6341,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D311" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E311" t="n">
         <v>0</v>
@@ -6477,10 +6477,10 @@
         <v>1</v>
       </c>
       <c r="D318" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">
@@ -6493,13 +6493,13 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D319" t="n">
         <v>0</v>
       </c>
       <c r="E319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320">
@@ -6512,13 +6512,13 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D320" t="n">
         <v>0</v>
       </c>
       <c r="E320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
@@ -6550,13 +6550,13 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D322" t="n">
         <v>0</v>
       </c>
       <c r="E322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323">
@@ -6588,13 +6588,13 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D324" t="n">
         <v>0</v>
       </c>
       <c r="E324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325">
@@ -6645,13 +6645,13 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D327" t="n">
         <v>0</v>
       </c>
       <c r="E327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328">
@@ -6721,10 +6721,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E331" t="n">
         <v>0</v>
@@ -6740,13 +6740,13 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D332" t="n">
         <v>0</v>
       </c>
       <c r="E332" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333">
@@ -6778,13 +6778,13 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D334" t="n">
         <v>0</v>
       </c>
       <c r="E334" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335">
@@ -6816,13 +6816,13 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D336" t="n">
         <v>0</v>
       </c>
       <c r="E336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337">
@@ -6930,13 +6930,13 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E342" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343">
@@ -6968,10 +6968,10 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D344" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E344" t="n">
         <v>0</v>
@@ -7006,13 +7006,13 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D346" t="n">
         <v>0</v>
       </c>
       <c r="E346" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="347">
@@ -7044,13 +7044,13 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D348" t="n">
         <v>0</v>
       </c>
       <c r="E348" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349">
@@ -7063,13 +7063,13 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D349" t="n">
         <v>0</v>
       </c>
       <c r="E349" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350">
@@ -7158,13 +7158,13 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D354" t="n">
         <v>0</v>
       </c>
       <c r="E354" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355">
@@ -7177,13 +7177,13 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D355" t="n">
         <v>0</v>
       </c>
       <c r="E355" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356">
@@ -7272,13 +7272,13 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D360" t="n">
         <v>0</v>
       </c>
       <c r="E360" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361">
@@ -7329,13 +7329,13 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D363" t="n">
         <v>0</v>
       </c>
       <c r="E363" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364">
@@ -7424,13 +7424,13 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D368" t="n">
         <v>0</v>
       </c>
       <c r="E368" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="369">
@@ -7481,13 +7481,13 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D371" t="n">
         <v>0</v>
       </c>
       <c r="E371" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372">
@@ -7538,13 +7538,13 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D374" t="n">
         <v>0</v>
       </c>
       <c r="E374" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="375">
@@ -7690,13 +7690,13 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D382" t="n">
         <v>0</v>
       </c>
       <c r="E382" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="383">
@@ -7709,13 +7709,13 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D383" t="n">
         <v>0</v>
       </c>
       <c r="E383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384">
@@ -7823,13 +7823,13 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D389" t="n">
         <v>0</v>
       </c>
       <c r="E389" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="390">
@@ -7861,13 +7861,13 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D391" t="n">
         <v>0</v>
       </c>
       <c r="E391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392">
@@ -7899,13 +7899,13 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D393" t="n">
         <v>0</v>
       </c>
       <c r="E393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
@@ -7918,13 +7918,13 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D394" t="n">
         <v>0</v>
       </c>
       <c r="E394" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
@@ -8035,10 +8035,10 @@
         <v>1</v>
       </c>
       <c r="D400" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E400" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401">
@@ -8089,13 +8089,13 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D403" t="n">
         <v>0</v>
       </c>
       <c r="E403" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404">
@@ -8127,13 +8127,13 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D405" t="n">
         <v>0</v>
       </c>
       <c r="E405" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406">
@@ -8184,13 +8184,13 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D408" t="n">
         <v>0</v>
       </c>
       <c r="E408" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="409">
@@ -8222,13 +8222,13 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D410" t="n">
         <v>0</v>
       </c>
       <c r="E410" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="411">
@@ -8241,13 +8241,13 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D411" t="n">
         <v>0</v>
       </c>
       <c r="E411" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412">
@@ -8279,13 +8279,13 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D413" t="n">
         <v>0</v>
       </c>
       <c r="E413" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414">
@@ -8317,10 +8317,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D415" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E415" t="n">
         <v>1</v>
@@ -8355,13 +8355,13 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D417" t="n">
         <v>0</v>
       </c>
       <c r="E417" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418">
@@ -8412,13 +8412,13 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D420" t="n">
         <v>0</v>
       </c>
       <c r="E420" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="421">
@@ -8450,13 +8450,13 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D422" t="n">
         <v>0</v>
       </c>
       <c r="E422" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="423">
@@ -8526,13 +8526,13 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D426" t="n">
         <v>0</v>
       </c>
       <c r="E426" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="427">
@@ -8545,13 +8545,13 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D427" t="n">
         <v>0</v>
       </c>
       <c r="E427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428">
@@ -8602,13 +8602,13 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D430" t="n">
         <v>0</v>
       </c>
       <c r="E430" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="431">
@@ -8640,13 +8640,13 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D432" t="n">
         <v>0</v>
       </c>
       <c r="E432" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433">
@@ -8697,13 +8697,13 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D435" t="n">
         <v>0</v>
       </c>
       <c r="E435" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436">
@@ -8716,13 +8716,13 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437">
@@ -8754,10 +8754,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D438" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E438" t="n">
         <v>0</v>
@@ -8792,10 +8792,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E440" t="n">
         <v>0</v>
@@ -8811,13 +8811,13 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D441" t="n">
         <v>0</v>
       </c>
       <c r="E441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442">
@@ -8830,10 +8830,10 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D442" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E442" t="n">
         <v>0</v>
@@ -8906,13 +8906,13 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D446" t="n">
         <v>0</v>
       </c>
       <c r="E446" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="447">
@@ -8944,13 +8944,13 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D448" t="n">
         <v>0</v>
       </c>
       <c r="E448" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="449">
@@ -8982,10 +8982,10 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E450" t="n">
         <v>0</v>
@@ -9134,13 +9134,13 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D458" t="n">
         <v>0</v>
       </c>
       <c r="E458" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459">
@@ -9153,13 +9153,13 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D459" t="n">
         <v>0</v>
       </c>
       <c r="E459" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="460">
@@ -9191,13 +9191,13 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D461" t="n">
         <v>0</v>
       </c>
       <c r="E461" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="462">
@@ -9229,10 +9229,10 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D463" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E463" t="n">
         <v>0</v>
@@ -9289,10 +9289,10 @@
         <v>1</v>
       </c>
       <c r="D466" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E466" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="467">
@@ -9343,13 +9343,13 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D469" t="n">
         <v>0</v>
       </c>
       <c r="E469" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="470">
@@ -9476,13 +9476,13 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D476" t="n">
         <v>0</v>
       </c>
       <c r="E476" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="477">
@@ -9495,10 +9495,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D477" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E477" t="n">
         <v>0</v>
@@ -9552,13 +9552,13 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D480" t="n">
         <v>0</v>
       </c>
       <c r="E480" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="481">
@@ -9571,13 +9571,13 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D481" t="n">
         <v>0</v>
       </c>
       <c r="E481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482">
@@ -9590,13 +9590,13 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D482" t="n">
         <v>0</v>
       </c>
       <c r="E482" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="483">
@@ -9723,13 +9723,13 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D489" t="n">
         <v>0</v>
       </c>
       <c r="E489" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="490">
@@ -9799,13 +9799,13 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D493" t="n">
         <v>0</v>
       </c>
       <c r="E493" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="494">
@@ -9818,13 +9818,13 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D494" t="n">
         <v>0</v>
       </c>
       <c r="E494" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="495">
@@ -9837,13 +9837,13 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D495" t="n">
         <v>0</v>
       </c>
       <c r="E495" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="496">
@@ -9856,13 +9856,13 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D496" t="n">
         <v>0</v>
       </c>
       <c r="E496" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="497">
@@ -10084,13 +10084,13 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D508" t="n">
         <v>0</v>
       </c>
       <c r="E508" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509">
@@ -10160,13 +10160,13 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D512" t="n">
         <v>0</v>
       </c>
       <c r="E512" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513">
@@ -10179,10 +10179,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D513" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E513" t="n">
         <v>0</v>
@@ -10198,13 +10198,13 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D514" t="n">
         <v>0</v>
       </c>
       <c r="E514" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="515">
@@ -10217,13 +10217,13 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D515" t="n">
         <v>0</v>
       </c>
       <c r="E515" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="516">
@@ -10255,13 +10255,13 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D517" t="n">
         <v>0</v>
       </c>
       <c r="E517" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="518">
@@ -10293,13 +10293,13 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D519" t="n">
         <v>0</v>
       </c>
       <c r="E519" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="520">
@@ -10331,13 +10331,13 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D521" t="n">
         <v>0</v>
       </c>
       <c r="E521" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="522">
@@ -10350,10 +10350,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D522" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E522" t="n">
         <v>1</v>
@@ -10483,13 +10483,13 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D529" t="n">
         <v>0</v>
       </c>
       <c r="E529" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="530">
@@ -10502,13 +10502,13 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D530" t="n">
         <v>0</v>
       </c>
       <c r="E530" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="531">
@@ -10597,10 +10597,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D535" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E535" t="n">
         <v>0</v>
@@ -10616,13 +10616,13 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D536" t="n">
         <v>0</v>
       </c>
       <c r="E536" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="537">
@@ -10711,10 +10711,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D541" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E541" t="n">
         <v>0</v>
@@ -10730,13 +10730,13 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D542" t="n">
         <v>0</v>
       </c>
       <c r="E542" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="543">
@@ -10806,13 +10806,13 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D546" t="n">
         <v>0</v>
       </c>
       <c r="E546" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="547">
@@ -10844,13 +10844,13 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D548" t="n">
         <v>0</v>
       </c>
       <c r="E548" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="549">
@@ -10863,13 +10863,13 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D549" t="n">
         <v>0</v>
       </c>
       <c r="E549" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="550">
@@ -10958,13 +10958,13 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D554" t="n">
         <v>0</v>
       </c>
       <c r="E554" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="555">
@@ -10996,13 +10996,13 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D556" t="n">
         <v>0</v>
       </c>
       <c r="E556" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="557">
@@ -11015,13 +11015,13 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D557" t="n">
         <v>0</v>
       </c>
       <c r="E557" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="558">
@@ -11091,13 +11091,13 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D561" t="n">
         <v>0</v>
       </c>
       <c r="E561" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="562">
@@ -11129,13 +11129,13 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D563" t="n">
         <v>0</v>
       </c>
       <c r="E563" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="564">
@@ -11148,10 +11148,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D564" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E564" t="n">
         <v>0</v>
@@ -11300,13 +11300,13 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D572" t="n">
         <v>0</v>
       </c>
       <c r="E572" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="573">
@@ -11357,13 +11357,13 @@
         </is>
       </c>
       <c r="C575" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D575" t="n">
         <v>0</v>
       </c>
       <c r="E575" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="576">
@@ -11376,13 +11376,13 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D576" t="n">
         <v>0</v>
       </c>
       <c r="E576" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="577">
@@ -11395,13 +11395,13 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D577" t="n">
         <v>0</v>
       </c>
       <c r="E577" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="578">
@@ -11414,10 +11414,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D578" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E578" t="n">
         <v>0</v>
@@ -11452,13 +11452,13 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D580" t="n">
         <v>0</v>
       </c>
       <c r="E580" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="581">
@@ -11490,10 +11490,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D582" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E582" t="n">
         <v>0</v>
@@ -11509,13 +11509,13 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D583" t="n">
         <v>0</v>
       </c>
       <c r="E583" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="584">
@@ -11528,13 +11528,13 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D584" t="n">
         <v>0</v>
       </c>
       <c r="E584" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="585">
@@ -11585,13 +11585,13 @@
         </is>
       </c>
       <c r="C587" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D587" t="n">
         <v>0</v>
       </c>
       <c r="E587" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="588">
@@ -11642,10 +11642,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D590" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E590" t="n">
         <v>0</v>
@@ -11737,13 +11737,13 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D595" t="n">
         <v>0</v>
       </c>
       <c r="E595" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="596">
@@ -11813,13 +11813,13 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D599" t="n">
         <v>0</v>
       </c>
       <c r="E599" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="600">
@@ -11851,13 +11851,13 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D601" t="n">
         <v>0</v>
       </c>
       <c r="E601" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="602">
@@ -11946,13 +11946,13 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D606" t="n">
         <v>0</v>
       </c>
       <c r="E606" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="607">
@@ -12022,13 +12022,13 @@
         </is>
       </c>
       <c r="C610" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D610" t="n">
         <v>0</v>
       </c>
       <c r="E610" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="611">
@@ -12060,13 +12060,13 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D612" t="n">
         <v>0</v>
       </c>
       <c r="E612" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613">
@@ -12079,13 +12079,13 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D613" t="n">
         <v>0</v>
       </c>
       <c r="E613" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="614">
@@ -12136,10 +12136,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D616" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E616" t="n">
         <v>0</v>
@@ -12155,13 +12155,13 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D617" t="n">
         <v>0</v>
       </c>
       <c r="E617" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="618">
@@ -12402,13 +12402,13 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D630" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E630" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="631">
@@ -12478,13 +12478,13 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D634" t="n">
         <v>0</v>
       </c>
       <c r="E634" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="635">
@@ -12535,13 +12535,13 @@
         </is>
       </c>
       <c r="C637" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D637" t="n">
         <v>0</v>
       </c>
       <c r="E637" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="638">
@@ -12630,13 +12630,13 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D642" t="n">
         <v>0</v>
       </c>
       <c r="E642" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="643">
@@ -12668,13 +12668,13 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D644" t="n">
         <v>0</v>
       </c>
       <c r="E644" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="645">
@@ -12744,13 +12744,13 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D648" t="n">
         <v>0</v>
       </c>
       <c r="E648" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="649">
@@ -12915,10 +12915,10 @@
         </is>
       </c>
       <c r="C657" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D657" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E657" t="n">
         <v>0</v>
@@ -12934,10 +12934,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D658" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E658" t="n">
         <v>0</v>
@@ -12953,13 +12953,13 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D659" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E659" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="660">
@@ -12991,13 +12991,13 @@
         </is>
       </c>
       <c r="C661" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D661" t="n">
         <v>0</v>
       </c>
       <c r="E661" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="662">
@@ -13086,13 +13086,13 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D666" t="n">
         <v>0</v>
       </c>
       <c r="E666" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="667">
@@ -13219,10 +13219,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D673" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E673" t="n">
         <v>0</v>
@@ -13238,13 +13238,13 @@
         </is>
       </c>
       <c r="C674" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D674" t="n">
         <v>0</v>
       </c>
       <c r="E674" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="675">
@@ -13333,13 +13333,13 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D679" t="n">
         <v>0</v>
       </c>
       <c r="E679" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="680">
@@ -13390,13 +13390,13 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D682" t="n">
         <v>0</v>
       </c>
       <c r="E682" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="683">
@@ -13447,13 +13447,13 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D685" t="n">
         <v>0</v>
       </c>
       <c r="E685" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="686">
@@ -13488,10 +13488,10 @@
         <v>1</v>
       </c>
       <c r="D687" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E687" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="688">
@@ -13618,13 +13618,13 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D694" t="n">
         <v>0</v>
       </c>
       <c r="E694" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="695">
@@ -13694,13 +13694,13 @@
         </is>
       </c>
       <c r="C698" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D698" t="n">
         <v>0</v>
       </c>
       <c r="E698" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="699">
@@ -13732,13 +13732,13 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D700" t="n">
         <v>0</v>
       </c>
       <c r="E700" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="701">
@@ -13751,13 +13751,13 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D701" t="n">
         <v>0</v>
       </c>
       <c r="E701" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="702">
@@ -13770,13 +13770,13 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D702" t="n">
         <v>0</v>
       </c>
       <c r="E702" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="703">
@@ -13846,13 +13846,13 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D706" t="n">
         <v>0</v>
       </c>
       <c r="E706" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="707">
@@ -13960,10 +13960,10 @@
         </is>
       </c>
       <c r="C712" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D712" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E712" t="n">
         <v>0</v>
@@ -14017,10 +14017,10 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D715" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E715" t="n">
         <v>0</v>
@@ -14055,13 +14055,13 @@
         </is>
       </c>
       <c r="C717" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D717" t="n">
         <v>0</v>
       </c>
       <c r="E717" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="718">
@@ -14112,13 +14112,13 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D720" t="n">
         <v>0</v>
       </c>
       <c r="E720" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="721">
@@ -14226,13 +14226,13 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D726" t="n">
         <v>0</v>
       </c>
       <c r="E726" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="727">
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C730" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D730" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E730" t="n">
         <v>0</v>
@@ -14378,13 +14378,13 @@
         </is>
       </c>
       <c r="C734" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D734" t="n">
         <v>0</v>
       </c>
       <c r="E734" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="735">
@@ -14435,10 +14435,10 @@
         </is>
       </c>
       <c r="C737" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D737" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E737" t="n">
         <v>0</v>
@@ -14568,13 +14568,13 @@
         </is>
       </c>
       <c r="C744" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D744" t="n">
         <v>0</v>
       </c>
       <c r="E744" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="745">
@@ -14625,10 +14625,10 @@
         </is>
       </c>
       <c r="C747" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D747" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E747" t="n">
         <v>0</v>
@@ -14682,10 +14682,10 @@
         </is>
       </c>
       <c r="C750" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D750" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E750" t="n">
         <v>0</v>
@@ -14796,13 +14796,13 @@
         </is>
       </c>
       <c r="C756" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D756" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E756" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="757">
@@ -14929,13 +14929,13 @@
         </is>
       </c>
       <c r="C763" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D763" t="n">
         <v>0</v>
       </c>
       <c r="E763" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="764">
@@ -15005,13 +15005,13 @@
         </is>
       </c>
       <c r="C767" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D767" t="n">
         <v>0</v>
       </c>
       <c r="E767" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="768">
@@ -15233,13 +15233,13 @@
         </is>
       </c>
       <c r="C779" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D779" t="n">
         <v>0</v>
       </c>
       <c r="E779" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="780">
@@ -15309,13 +15309,13 @@
         </is>
       </c>
       <c r="C783" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D783" t="n">
         <v>0</v>
       </c>
       <c r="E783" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784">
@@ -15347,13 +15347,13 @@
         </is>
       </c>
       <c r="C785" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D785" t="n">
         <v>0</v>
       </c>
       <c r="E785" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="786">
@@ -15366,13 +15366,13 @@
         </is>
       </c>
       <c r="C786" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D786" t="n">
         <v>0</v>
       </c>
       <c r="E786" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="787">
@@ -15442,13 +15442,13 @@
         </is>
       </c>
       <c r="C790" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D790" t="n">
         <v>0</v>
       </c>
       <c r="E790" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="791">
@@ -15461,10 +15461,10 @@
         </is>
       </c>
       <c r="C791" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D791" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E791" t="n">
         <v>0</v>
@@ -15556,10 +15556,10 @@
         </is>
       </c>
       <c r="C796" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D796" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E796" t="n">
         <v>0</v>
@@ -15803,13 +15803,13 @@
         </is>
       </c>
       <c r="C809" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D809" t="n">
         <v>0</v>
       </c>
       <c r="E809" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="810">
@@ -15822,10 +15822,10 @@
         </is>
       </c>
       <c r="C810" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D810" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E810" t="n">
         <v>0</v>
@@ -15841,13 +15841,13 @@
         </is>
       </c>
       <c r="C811" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D811" t="n">
         <v>0</v>
       </c>
       <c r="E811" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="812">
@@ -15860,10 +15860,10 @@
         </is>
       </c>
       <c r="C812" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D812" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E812" t="n">
         <v>0</v>
@@ -16107,10 +16107,10 @@
         </is>
       </c>
       <c r="C825" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D825" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E825" t="n">
         <v>0</v>
@@ -16278,13 +16278,13 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D834" t="n">
         <v>0</v>
       </c>
       <c r="E834" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="835">
@@ -16335,13 +16335,13 @@
         </is>
       </c>
       <c r="C837" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D837" t="n">
         <v>0</v>
       </c>
       <c r="E837" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="838">
@@ -16354,13 +16354,13 @@
         </is>
       </c>
       <c r="C838" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D838" t="n">
         <v>0</v>
       </c>
       <c r="E838" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="839">
@@ -16373,13 +16373,13 @@
         </is>
       </c>
       <c r="C839" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D839" t="n">
         <v>0</v>
       </c>
       <c r="E839" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="840">
@@ -16468,10 +16468,10 @@
         </is>
       </c>
       <c r="C844" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D844" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E844" t="n">
         <v>0</v>
@@ -16509,10 +16509,10 @@
         <v>1</v>
       </c>
       <c r="D846" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E846" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="847">
@@ -16525,13 +16525,13 @@
         </is>
       </c>
       <c r="C847" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D847" t="n">
         <v>0</v>
       </c>
       <c r="E847" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="848">
@@ -16582,13 +16582,13 @@
         </is>
       </c>
       <c r="C850" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D850" t="n">
         <v>0</v>
       </c>
       <c r="E850" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="851">
@@ -16753,13 +16753,13 @@
         </is>
       </c>
       <c r="C859" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D859" t="n">
         <v>0</v>
       </c>
       <c r="E859" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="860">
@@ -16848,13 +16848,13 @@
         </is>
       </c>
       <c r="C864" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D864" t="n">
         <v>0</v>
       </c>
       <c r="E864" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="865">
@@ -16924,10 +16924,10 @@
         </is>
       </c>
       <c r="C868" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D868" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E868" t="n">
         <v>0</v>
@@ -17000,13 +17000,13 @@
         </is>
       </c>
       <c r="C872" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D872" t="n">
         <v>0</v>
       </c>
       <c r="E872" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="873">
@@ -17057,13 +17057,13 @@
         </is>
       </c>
       <c r="C875" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D875" t="n">
         <v>0</v>
       </c>
       <c r="E875" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="876">
@@ -17133,13 +17133,13 @@
         </is>
       </c>
       <c r="C879" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D879" t="n">
         <v>0</v>
       </c>
       <c r="E879" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="880">
@@ -17171,13 +17171,13 @@
         </is>
       </c>
       <c r="C881" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D881" t="n">
         <v>0</v>
       </c>
       <c r="E881" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="882">
@@ -17209,10 +17209,10 @@
         </is>
       </c>
       <c r="C883" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D883" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E883" t="n">
         <v>0</v>
@@ -17228,13 +17228,13 @@
         </is>
       </c>
       <c r="C884" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D884" t="n">
         <v>0</v>
       </c>
       <c r="E884" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="885">
@@ -17266,10 +17266,10 @@
         </is>
       </c>
       <c r="C886" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D886" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E886" t="n">
         <v>0</v>
@@ -17285,10 +17285,10 @@
         </is>
       </c>
       <c r="C887" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D887" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E887" t="n">
         <v>0</v>
@@ -17323,10 +17323,10 @@
         </is>
       </c>
       <c r="C889" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D889" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E889" t="n">
         <v>0</v>
@@ -17342,13 +17342,13 @@
         </is>
       </c>
       <c r="C890" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D890" t="n">
         <v>0</v>
       </c>
       <c r="E890" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="891">
@@ -17437,13 +17437,13 @@
         </is>
       </c>
       <c r="C895" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D895" t="n">
         <v>0</v>
       </c>
       <c r="E895" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="896">
@@ -17456,13 +17456,13 @@
         </is>
       </c>
       <c r="C896" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D896" t="n">
         <v>0</v>
       </c>
       <c r="E896" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="897">
@@ -17551,13 +17551,13 @@
         </is>
       </c>
       <c r="C901" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D901" t="n">
         <v>0</v>
       </c>
       <c r="E901" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="902">
@@ -17627,10 +17627,10 @@
         </is>
       </c>
       <c r="C905" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D905" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E905" t="n">
         <v>0</v>
@@ -17684,10 +17684,10 @@
         </is>
       </c>
       <c r="C908" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D908" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E908" t="n">
         <v>0</v>
@@ -17988,10 +17988,10 @@
         </is>
       </c>
       <c r="C924" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D924" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E924" t="n">
         <v>0</v>
@@ -18064,10 +18064,10 @@
         </is>
       </c>
       <c r="C928" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D928" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E928" t="n">
         <v>0</v>
@@ -18558,10 +18558,10 @@
         </is>
       </c>
       <c r="C954" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D954" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E954" t="n">
         <v>0</v>

</xml_diff>